<commit_message>
further flagging revisions to final draft for comgr review
</commit_message>
<xml_diff>
--- a/ca_pr_mu_flagged.xlsx
+++ b/ca_pr_mu_flagged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/coho/rrCoho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="8_{F782DFB3-929D-6B42-A858-9292F5F68A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9629724-22E1-B944-AD4E-297AB37C4356}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{F782DFB3-929D-6B42-A858-9292F5F68A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BDF6ACB-3409-A34E-93D5-952DCCE9259A}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="760" windowWidth="28320" windowHeight="17440" xr2:uid="{C4FCB720-54B6-7F4D-9244-5678EB8B5A54}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9149" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9160" uniqueCount="1111">
   <si>
     <t>area9w</t>
   </si>
@@ -3441,13 +3441,13 @@
     <t>6_8</t>
   </si>
   <si>
-    <t>removed CWT flag, because contribution seems too high</t>
-  </si>
-  <si>
     <t>use run path; CWT catch &gt; total</t>
   </si>
   <si>
-    <t>use runpath, cwtcatch&gt;catch</t>
+    <t>removed HR &amp; CWT flag, because contribution seems too high</t>
+  </si>
+  <si>
+    <t>use runpath, CWTs erroneous H/W</t>
   </si>
 </sst>
 </file>
@@ -3877,8 +3877,8 @@
   <dimension ref="A1:M1801"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1313" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1304" sqref="F1304"/>
+      <pane ySplit="1" topLeftCell="A830" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1732" sqref="M1732"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30993,9 +30993,6 @@
       <c r="I896" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J896" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="897" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A897" s="1">
@@ -31024,12 +31021,6 @@
       </c>
       <c r="I897" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="J897" s="1">
-        <v>1</v>
-      </c>
-      <c r="K897" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="898" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -43412,12 +43403,8 @@
       <c r="I1273" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="J1273" s="3">
-        <v>1</v>
-      </c>
-      <c r="K1273" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1273" s="3"/>
+      <c r="K1273" s="3"/>
       <c r="L1273" s="3"/>
     </row>
     <row r="1274" spans="1:12" x14ac:dyDescent="0.2">
@@ -44614,9 +44601,7 @@
       <c r="I1310" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J1310" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1310" s="3"/>
       <c r="K1310" s="3"/>
       <c r="L1310" s="3"/>
     </row>
@@ -45040,12 +45025,8 @@
       <c r="I1323" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="J1323" s="3">
-        <v>1</v>
-      </c>
-      <c r="K1323" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1323" s="3"/>
+      <c r="K1323" s="3"/>
       <c r="L1323" s="3"/>
     </row>
     <row r="1324" spans="1:12" x14ac:dyDescent="0.2">
@@ -45076,9 +45057,7 @@
       <c r="I1324" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="J1324" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1324" s="3"/>
       <c r="K1324" s="3"/>
       <c r="L1324" s="3"/>
     </row>
@@ -47606,11 +47585,11 @@
       <c r="I1402" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J1402" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1402" s="3"/>
       <c r="K1402" s="3"/>
-      <c r="L1402" s="3"/>
+      <c r="L1402" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1403" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1403" s="3">
@@ -47640,11 +47619,11 @@
       <c r="I1403" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J1403" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1403" s="3"/>
       <c r="K1403" s="3"/>
-      <c r="L1403" s="3"/>
+      <c r="L1403" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1404" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1404" s="3">
@@ -47678,7 +47657,9 @@
         <v>1</v>
       </c>
       <c r="K1404" s="3"/>
-      <c r="L1404" s="3"/>
+      <c r="L1404" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1405" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1405" s="3">
@@ -47712,7 +47693,9 @@
         <v>1</v>
       </c>
       <c r="K1405" s="3"/>
-      <c r="L1405" s="3"/>
+      <c r="L1405" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1406" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1406" s="3">
@@ -47742,11 +47725,11 @@
       <c r="I1406" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J1406" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1406" s="3"/>
       <c r="K1406" s="3"/>
-      <c r="L1406" s="3"/>
+      <c r="L1406" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1407" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1407" s="3">
@@ -47780,7 +47763,9 @@
         <v>1</v>
       </c>
       <c r="K1407" s="3"/>
-      <c r="L1407" s="3"/>
+      <c r="L1407" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1408" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1408" s="3">
@@ -47814,7 +47799,9 @@
         <v>1</v>
       </c>
       <c r="K1408" s="3"/>
-      <c r="L1408" s="3"/>
+      <c r="L1408" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1409" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1409" s="3">
@@ -47844,11 +47831,11 @@
       <c r="I1409" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J1409" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1409" s="3"/>
       <c r="K1409" s="3"/>
-      <c r="L1409" s="3"/>
+      <c r="L1409" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1410" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1410" s="3">
@@ -47882,7 +47869,9 @@
         <v>1</v>
       </c>
       <c r="K1410" s="3"/>
-      <c r="L1410" s="3"/>
+      <c r="L1410" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1411" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1411" s="3">
@@ -47916,7 +47905,9 @@
         <v>1</v>
       </c>
       <c r="K1411" s="3"/>
-      <c r="L1411" s="3"/>
+      <c r="L1411" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1412" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1412" s="3">
@@ -47946,11 +47937,11 @@
       <c r="I1412" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J1412" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1412" s="3"/>
       <c r="K1412" s="3"/>
-      <c r="L1412" s="3"/>
+      <c r="L1412" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="1413" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1413" s="3">
@@ -49232,13 +49223,11 @@
       <c r="I1452" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J1452" s="3">
-        <v>1</v>
-      </c>
+      <c r="J1452" s="3"/>
       <c r="K1452" s="3"/>
       <c r="L1452" s="3"/>
       <c r="M1452" t="s">
-        <v>1108</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="1453" spans="1:13" x14ac:dyDescent="0.2">
@@ -51591,7 +51580,7 @@
       <c r="K1524" s="3"/>
       <c r="L1524" s="3"/>
       <c r="M1524" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1525" spans="1:13" x14ac:dyDescent="0.2">
@@ -51730,7 +51719,7 @@
       <c r="K1528" s="3"/>
       <c r="L1528" s="3"/>
       <c r="M1528" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1529" spans="1:13" x14ac:dyDescent="0.2">
@@ -51903,7 +51892,7 @@
       <c r="K1533" s="3"/>
       <c r="L1533" s="3"/>
       <c r="M1533" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1534" spans="1:13" x14ac:dyDescent="0.2">
@@ -52042,7 +52031,7 @@
       <c r="K1537" s="3"/>
       <c r="L1537" s="3"/>
       <c r="M1537" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1538" spans="1:13" x14ac:dyDescent="0.2">
@@ -52113,7 +52102,7 @@
       <c r="K1539" s="3"/>
       <c r="L1539" s="3"/>
       <c r="M1539" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="1540" spans="1:13" x14ac:dyDescent="0.2">
@@ -57877,9 +57866,7 @@
       <c r="J1716" s="3">
         <v>1</v>
       </c>
-      <c r="K1716" s="3">
-        <v>1</v>
-      </c>
+      <c r="K1716" s="3"/>
       <c r="L1716" s="3"/>
       <c r="M1716" t="s">
         <v>1110</v>
@@ -57916,9 +57903,7 @@
       <c r="J1717" s="3">
         <v>1</v>
       </c>
-      <c r="K1717" s="3">
-        <v>1</v>
-      </c>
+      <c r="K1717" s="3"/>
       <c r="L1717" s="3"/>
       <c r="M1717" t="s">
         <v>1110</v>
@@ -58023,9 +58008,7 @@
       <c r="J1720" s="3">
         <v>1</v>
       </c>
-      <c r="K1720" s="3">
-        <v>1</v>
-      </c>
+      <c r="K1720" s="3"/>
       <c r="L1720" s="3"/>
       <c r="M1720" t="s">
         <v>1110</v>
@@ -58198,9 +58181,7 @@
       <c r="J1725" s="3">
         <v>1</v>
       </c>
-      <c r="K1725" s="3">
-        <v>1</v>
-      </c>
+      <c r="K1725" s="3"/>
       <c r="L1725" s="3"/>
       <c r="M1725" t="s">
         <v>1110</v>
@@ -58339,9 +58320,7 @@
       <c r="J1729" s="3">
         <v>1</v>
       </c>
-      <c r="K1729" s="3">
-        <v>1</v>
-      </c>
+      <c r="K1729" s="3"/>
       <c r="L1729" s="3"/>
       <c r="M1729" t="s">
         <v>1110</v>
@@ -58412,9 +58391,7 @@
       <c r="J1731" s="3">
         <v>1</v>
       </c>
-      <c r="K1731" s="3">
-        <v>1</v>
-      </c>
+      <c r="K1731" s="3"/>
       <c r="L1731" s="3"/>
       <c r="M1731" t="s">
         <v>1110</v>
@@ -60544,9 +60521,7 @@
       <c r="I1796" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J1796" s="1">
-        <v>1</v>
-      </c>
+      <c r="J1796" s="1"/>
       <c r="K1796" s="1"/>
       <c r="L1796" s="1"/>
     </row>
@@ -60578,12 +60553,8 @@
       <c r="I1797" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1797" s="1">
-        <v>1</v>
-      </c>
-      <c r="K1797" s="1">
-        <v>1</v>
-      </c>
+      <c r="J1797" s="1"/>
+      <c r="K1797" s="1"/>
       <c r="L1797" s="1"/>
     </row>
     <row r="1798" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
final 2021 tweaks pre-Btable
</commit_message>
<xml_diff>
--- a/ca_pr_mu_flagged.xlsx
+++ b/ca_pr_mu_flagged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/daniel_auerbach_dfw_wa_gov/Documents/code/coho/rrCoho/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="8_{F782DFB3-929D-6B42-A858-9292F5F68A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BDF6ACB-3409-A34E-93D5-952DCCE9259A}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="8_{F782DFB3-929D-6B42-A858-9292F5F68A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B87B92E2-D05E-994E-8630-062B2CB97D3B}"/>
   <bookViews>
     <workbookView xWindow="620" yWindow="760" windowWidth="28320" windowHeight="17440" xr2:uid="{C4FCB720-54B6-7F4D-9244-5678EB8B5A54}"/>
   </bookViews>
@@ -3877,8 +3877,8 @@
   <dimension ref="A1:M1801"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A830" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1732" sqref="M1732"/>
+      <pane ySplit="1" topLeftCell="A981" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K985" sqref="K985"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33924,7 +33924,9 @@
       <c r="J984" s="5">
         <v>1</v>
       </c>
-      <c r="K984" s="5"/>
+      <c r="K984" s="5">
+        <v>1</v>
+      </c>
       <c r="L984" s="5" t="s">
         <v>63</v>
       </c>

</xml_diff>